<commit_message>
Add Debugger Add b_out, g_out, r_out, alpha_out
</commit_message>
<xml_diff>
--- a/Image processing pyqt5_Layout.xlsx
+++ b/Image processing pyqt5_Layout.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A\Desktop\pythonProject\opencvProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A\Desktop\pythonProject\Image_processing_pyqt5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D06167C-AC48-4EB8-BBF2-4BC2C18920C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75572558-C845-4125-B40B-CFD30AAD7AF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-140" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pdf2image_memo" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="87">
   <si>
     <t>main_layout</t>
     <phoneticPr fontId="1"/>
@@ -122,22 +122,10 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>b1_from</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>b1_to</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>g0_from</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>g1_to</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>r0_from</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -146,19 +134,7 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>r1_from</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>r1_to</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>g0_to</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>g1_from</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -457,27 +433,6 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>range_exe1</t>
-    </r>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Segoe UI Symbol"/>
-        <family val="2"/>
-      </rPr>
-      <t>☑</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
         <rFont val="Yu Gothic"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -487,10 +442,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t># Range conversion</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t># Point conversion</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -516,6 +467,54 @@
   </si>
   <si>
     <t># thread_count</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>: pdf -&gt; image (jpg/png/tif). Be careful with "grayscale" checkbox.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>: Convert all the pdf files to images in the directory (jpg/png/tif).</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>: Add filename1 on filename0 (tif -&gt; tif).</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>alpha</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>r_out</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>g_out</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>b_out</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>alpha_out</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&lt;lower&gt;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&lt;upper&gt;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&lt;out&gt;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t># Make selected color channel to arbitrary color. Only works for output: .png/.tif.</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -808,31 +807,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1160,12 +1148,12 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75"/>
+  <sheetFormatPr defaultRowHeight="18"/>
   <cols>
     <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="14.125" customWidth="1"/>
-    <col min="5" max="5" width="14.625" customWidth="1"/>
-    <col min="6" max="6" width="14.875" customWidth="1"/>
+    <col min="4" max="4" width="14.08203125" customWidth="1"/>
+    <col min="5" max="5" width="14.58203125" customWidth="1"/>
+    <col min="6" max="6" width="14.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:6">
@@ -1202,7 +1190,7 @@
     </row>
     <row r="8" spans="2:6">
       <c r="B8" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="2:6">
@@ -1232,258 +1220,265 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE5F4307-24ED-4B12-88F6-644A1CFE48C2}">
   <dimension ref="C4:L23"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="18.75"/>
+  <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="18"/>
   <sheetData>
     <row r="4" spans="3:12">
       <c r="C4" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="5" spans="3:12" ht="19.5" thickBot="1">
-      <c r="C5" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D5" s="3"/>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="3:12" ht="18.5" thickBot="1">
+      <c r="C5" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="6" spans="3:12">
-      <c r="C6" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="D6" s="19"/>
+      <c r="C6" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="12"/>
+      <c r="E6" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="7" spans="3:12">
-      <c r="C7" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="D7" s="21"/>
-    </row>
-    <row r="8" spans="3:12" ht="19.5" thickBot="1">
-      <c r="C8" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="D8" s="23"/>
-    </row>
-    <row r="9" spans="3:12" ht="19.5" thickBot="1">
-      <c r="C9" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="D9" s="23"/>
+      <c r="C7" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="14"/>
+      <c r="E7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="3:12" ht="18.5" thickBot="1">
+      <c r="C8" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="16"/>
+      <c r="E8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" spans="3:12" ht="18.5" thickBot="1">
+      <c r="C9" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" s="16"/>
+      <c r="E9" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="11" spans="3:12">
       <c r="C11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="3:12" ht="18.5" thickBot="1">
+      <c r="C12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="3:12" ht="18.5" thickBot="1">
+      <c r="C13" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="18"/>
+      <c r="J13" s="18"/>
+      <c r="K13" s="19"/>
+      <c r="L13" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="3:12" ht="18.5" thickBot="1">
+      <c r="C14" s="4">
+        <v>100</v>
+      </c>
+      <c r="D14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="3:12" ht="18.5" thickBot="1"/>
+    <row r="16" spans="3:12" ht="18.5" thickBot="1">
+      <c r="C16" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="K11" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="L11" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="12" spans="3:12" ht="19.5" thickBot="1">
-      <c r="C12" t="s">
+      <c r="D16" s="18"/>
+      <c r="E16" s="19"/>
+      <c r="F16" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="13" spans="3:12" ht="19.5" thickBot="1">
-      <c r="C13" s="24" t="s">
+      <c r="G16" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="H16" s="18"/>
+      <c r="I16" s="19"/>
+      <c r="J16" t="s">
         <v>39</v>
-      </c>
-      <c r="D13" s="25"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="25"/>
-      <c r="G13" s="25"/>
-      <c r="H13" s="25"/>
-      <c r="I13" s="25"/>
-      <c r="J13" s="25"/>
-      <c r="K13" s="26"/>
-      <c r="L13" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="14" spans="3:12" ht="19.5" thickBot="1">
-      <c r="C14" s="5">
-        <v>100</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="F14" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="15" spans="3:12" ht="19.5" thickBot="1">
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-    </row>
-    <row r="16" spans="3:12" ht="19.5" thickBot="1">
-      <c r="C16" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="D16" s="25"/>
-      <c r="E16" s="26"/>
-      <c r="F16" t="s">
-        <v>44</v>
-      </c>
-      <c r="G16" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="H16" s="25"/>
-      <c r="I16" s="26"/>
-      <c r="J16" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="18" spans="3:12">
       <c r="C18" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="3:12" ht="18.5" thickBot="1">
+      <c r="C19" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="3:12" ht="18.5" thickBot="1">
+      <c r="C20" t="s">
+        <v>42</v>
+      </c>
+      <c r="E20" s="4">
+        <v>1</v>
+      </c>
+      <c r="F20" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="21" spans="3:12" ht="18.5" thickBot="1">
+      <c r="C21" t="s">
+        <v>43</v>
+      </c>
+      <c r="H21" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="3:12" ht="18.5" thickBot="1">
+      <c r="D22" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="E22" s="4">
+        <v>1</v>
+      </c>
+      <c r="F22" t="s">
         <v>57</v>
       </c>
-      <c r="E18" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="K18" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="L18" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="19" spans="3:12" ht="19.5" thickBot="1">
-      <c r="C19" t="s">
+      <c r="I22" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="J22" s="4">
+        <v>9999</v>
+      </c>
+      <c r="K22" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="23" spans="3:12" ht="18.5" thickBot="1">
+      <c r="D23" s="5" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="20" spans="3:12" ht="19.5" thickBot="1">
-      <c r="C20" t="s">
-        <v>48</v>
-      </c>
-      <c r="E20" s="5">
-        <v>1</v>
-      </c>
-      <c r="F20" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="21" spans="3:12" ht="19.5" thickBot="1">
-      <c r="C21" t="s">
+      <c r="E23" s="4">
+        <v>2</v>
+      </c>
+      <c r="F23" t="s">
+        <v>58</v>
+      </c>
+      <c r="I23" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="H21" s="11" t="s">
+      <c r="J23" s="4">
+        <v>9999</v>
+      </c>
+      <c r="K23" t="s">
         <v>56</v>
-      </c>
-    </row>
-    <row r="22" spans="3:12" ht="19.5" thickBot="1">
-      <c r="D22" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="E22" s="5">
-        <v>1</v>
-      </c>
-      <c r="F22" t="s">
-        <v>63</v>
-      </c>
-      <c r="I22" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="J22" s="7">
-        <v>9999</v>
-      </c>
-      <c r="K22" s="8" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="23" spans="3:12" ht="19.5" thickBot="1">
-      <c r="D23" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="E23" s="5">
-        <v>2</v>
-      </c>
-      <c r="F23" t="s">
-        <v>64</v>
-      </c>
-      <c r="I23" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="J23" s="7">
-        <v>9999</v>
-      </c>
-      <c r="K23" s="8" t="s">
-        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1504,254 +1499,253 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8435DF8B-284E-40B4-AEA6-EB65CAC52314}">
-  <dimension ref="C2:L20"/>
+  <dimension ref="C2:L19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="18.75"/>
+  <sheetFormatPr defaultColWidth="12.58203125" defaultRowHeight="18"/>
   <sheetData>
     <row r="2" spans="3:12">
       <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="3" spans="3:12" ht="19.5" thickBot="1">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="3:12" ht="18.5" thickBot="1">
       <c r="C3" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="3:12" ht="19.5" thickBot="1">
-      <c r="C4" s="28" t="s">
-        <v>60</v>
-      </c>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="29"/>
-      <c r="H4" s="29"/>
-      <c r="I4" s="29"/>
-      <c r="J4" s="29"/>
-      <c r="K4" s="30"/>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="3:12" ht="18.5" thickBot="1">
+      <c r="C4" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="22"/>
+      <c r="J4" s="22"/>
+      <c r="K4" s="23"/>
       <c r="L4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="5" spans="3:12" ht="19.5" thickBot="1">
-      <c r="C5" s="15" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="3:12" ht="18.5" thickBot="1">
+      <c r="C5" s="9" t="s">
         <v>8</v>
       </c>
       <c r="D5" t="s">
         <v>9</v>
       </c>
       <c r="L5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="6" spans="3:12" ht="19.5" thickBot="1">
-      <c r="D6" s="5"/>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="3:12" ht="18.5" thickBot="1">
+      <c r="D6" s="4"/>
       <c r="E6" t="s">
-        <v>81</v>
-      </c>
-      <c r="J6" s="6"/>
+        <v>73</v>
+      </c>
     </row>
     <row r="7" spans="3:12">
-      <c r="C7" s="17" t="s">
-        <v>79</v>
+      <c r="C7" s="10" t="s">
+        <v>71</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="3:12">
-      <c r="C8" s="9"/>
-      <c r="D8" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="E8" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="F8" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="G8" s="14" t="s">
+      <c r="C8" s="5"/>
+      <c r="D8" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="3:12">
+      <c r="C9" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="3:12">
+      <c r="C10" s="5"/>
+      <c r="D10" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="3:12">
+      <c r="C11" s="10" t="s">
         <v>69</v>
-      </c>
-    </row>
-    <row r="9" spans="3:12">
-      <c r="C9" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="L9" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="10" spans="3:12">
-      <c r="C10" s="9"/>
-      <c r="D10" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="E10" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="F10" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="G10" s="14" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="11" spans="3:12">
-      <c r="C11" s="16" t="s">
-        <v>77</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="12" spans="3:12" ht="19.5" thickBot="1">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="3:12" ht="18.5" thickBot="1">
       <c r="C12" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="13" spans="3:12" ht="19.5" thickBot="1">
-      <c r="C13" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="E13" s="13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="3:12" ht="18.5" thickBot="1">
+      <c r="C13" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E13" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F13" t="s">
         <v>10</v>
       </c>
-      <c r="G13" s="12" t="s">
+      <c r="G13" s="6" t="s">
         <v>15</v>
       </c>
       <c r="H13" t="s">
         <v>11</v>
       </c>
-      <c r="I13" s="12" t="s">
+      <c r="I13" s="6" t="s">
         <v>17</v>
       </c>
       <c r="J13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="3:12" ht="19.5" thickBot="1">
-      <c r="C14" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="E14" s="12" t="s">
+    <row r="14" spans="3:12" ht="18.5" thickBot="1">
+      <c r="C14" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E14" s="6" t="s">
         <v>13</v>
       </c>
       <c r="F14" t="s">
         <v>10</v>
       </c>
-      <c r="G14" s="12" t="s">
+      <c r="G14" s="6" t="s">
         <v>16</v>
       </c>
       <c r="H14" t="s">
         <v>11</v>
       </c>
-      <c r="I14" s="12" t="s">
+      <c r="I14" s="6" t="s">
         <v>18</v>
       </c>
       <c r="J14" t="s">
@@ -1759,136 +1753,117 @@
       </c>
     </row>
     <row r="15" spans="3:12">
-      <c r="C15" s="16" t="s">
-        <v>78</v>
+      <c r="C15" s="10" t="s">
+        <v>70</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="16" spans="3:12" ht="19.5" thickBot="1">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="3:12" ht="18.5" thickBot="1">
       <c r="C16" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="17" spans="3:10" ht="19.5" thickBot="1">
-      <c r="C17" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="E17" s="12" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="17" spans="3:12" ht="18.5" thickBot="1">
+      <c r="C17" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="E17" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F17" t="s">
         <v>10</v>
       </c>
-      <c r="G17" s="12" t="s">
-        <v>23</v>
+      <c r="G17" s="6" t="s">
+        <v>21</v>
       </c>
       <c r="H17" t="s">
         <v>11</v>
       </c>
-      <c r="I17" s="12" t="s">
-        <v>25</v>
+      <c r="I17" s="6" t="s">
+        <v>22</v>
       </c>
       <c r="J17" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="3:10" ht="19.5" thickBot="1">
-      <c r="D18" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="E18" s="12" t="s">
+    <row r="18" spans="3:12" ht="18.5" thickBot="1">
+      <c r="D18" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="E18" s="6" t="s">
         <v>20</v>
       </c>
       <c r="F18" t="s">
         <v>10</v>
       </c>
-      <c r="G18" s="12" t="s">
-        <v>29</v>
+      <c r="G18" s="6" t="s">
+        <v>24</v>
       </c>
       <c r="H18" t="s">
         <v>11</v>
       </c>
-      <c r="I18" s="12" t="s">
-        <v>26</v>
+      <c r="I18" s="6" t="s">
+        <v>23</v>
       </c>
       <c r="J18" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="3:10" ht="19.5" thickBot="1">
-      <c r="C19" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="E19" s="12" t="s">
-        <v>21</v>
+    <row r="19" spans="3:12" ht="18.5" thickBot="1">
+      <c r="C19" s="3"/>
+      <c r="D19" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>81</v>
       </c>
       <c r="F19" t="s">
         <v>10</v>
       </c>
-      <c r="G19" s="12" t="s">
-        <v>30</v>
+      <c r="G19" s="6" t="s">
+        <v>80</v>
       </c>
       <c r="H19" t="s">
         <v>11</v>
       </c>
-      <c r="I19" s="12" t="s">
-        <v>27</v>
+      <c r="I19" s="6" t="s">
+        <v>79</v>
       </c>
       <c r="J19" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="20" spans="3:10" ht="19.5" thickBot="1">
-      <c r="D20" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="E20" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="F20" t="s">
-        <v>10</v>
-      </c>
-      <c r="G20" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="H20" t="s">
-        <v>11</v>
-      </c>
-      <c r="I20" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="J20" t="s">
-        <v>12</v>
+      <c r="K19" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="L19" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add BGR spin box for add_image_tif (b2,g2,r2,b3,g3,r3). v01.01.01.
</commit_message>
<xml_diff>
--- a/Image processing pyqt5_Layout.xlsx
+++ b/Image processing pyqt5_Layout.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A\Desktop\pythonProject\Image_processing_pyqt5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75572558-C845-4125-B40B-CFD30AAD7AF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBD2CBA3-EAF0-4284-9C2A-A30DDCBD7C87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pdf2image_memo" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="96">
   <si>
     <t>main_layout</t>
     <phoneticPr fontId="1"/>
@@ -515,6 +515,42 @@
   </si>
   <si>
     <t># Make selected color channel to arbitrary color. Only works for output: .png/.tif.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t># filename :filename used for pdf2image</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>BGR</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>---&gt;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>b2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>g2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>r2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>b3</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>g3</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>r3</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -807,7 +843,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -841,9 +877,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -860,6 +893,31 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1218,10 +1276,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE5F4307-24ED-4B12-88F6-644A1CFE48C2}">
-  <dimension ref="C4:L23"/>
+  <dimension ref="C4:L26"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="18"/>
@@ -1337,159 +1395,201 @@
       </c>
     </row>
     <row r="13" spans="3:12" ht="18.5" thickBot="1">
-      <c r="C13" s="17" t="s">
+      <c r="C13" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="18"/>
-      <c r="I13" s="18"/>
-      <c r="J13" s="18"/>
-      <c r="K13" s="19"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="28"/>
+      <c r="H13" t="s">
+        <v>53</v>
+      </c>
+      <c r="I13" s="4">
+        <v>100</v>
+      </c>
+      <c r="J13" t="s">
+        <v>34</v>
+      </c>
+      <c r="K13" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="L13" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="14" spans="3:12" ht="18.5" thickBot="1">
-      <c r="C14" s="4">
-        <v>100</v>
-      </c>
-      <c r="D14" t="s">
-        <v>34</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="F14" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="15" spans="3:12" ht="18.5" thickBot="1"/>
     <row r="16" spans="3:12" ht="18.5" thickBot="1">
-      <c r="C16" s="20" t="s">
+      <c r="C16" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="D16" s="18"/>
-      <c r="E16" s="19"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="18"/>
       <c r="F16" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="17" spans="3:12" ht="18.5" thickBot="1">
+      <c r="C17" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" s="17"/>
+      <c r="E17" s="18"/>
+      <c r="F17" t="s">
         <v>38</v>
       </c>
-      <c r="G16" s="17" t="s">
+      <c r="H17" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="H16" s="18"/>
-      <c r="I16" s="19"/>
-      <c r="J16" t="s">
+      <c r="I17" s="30"/>
+      <c r="J17" s="31"/>
+      <c r="K17" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="3:12">
-      <c r="C18" t="s">
+    <row r="18" spans="3:12" ht="18.5" thickBot="1">
+      <c r="C18" s="23"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="24"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="24"/>
+    </row>
+    <row r="19" spans="3:12" ht="18.5" thickBot="1">
+      <c r="C19" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F19" t="s">
+        <v>88</v>
+      </c>
+      <c r="G19" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="H19" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="J19" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="K19" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="21" spans="3:12">
+      <c r="C21" t="s">
         <v>40</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="K18" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="L18" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="19" spans="3:12" ht="18.5" thickBot="1">
-      <c r="C19" t="s">
+      <c r="D21" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="L21" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="3:12" ht="18.5" thickBot="1">
+      <c r="C22" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="3:12" ht="18.5" thickBot="1">
-      <c r="C20" t="s">
+    <row r="23" spans="3:12" ht="18.5" thickBot="1">
+      <c r="C23" t="s">
         <v>42</v>
       </c>
-      <c r="E20" s="4">
+      <c r="E23" s="4">
         <v>1</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F23" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="21" spans="3:12" ht="18.5" thickBot="1">
-      <c r="C21" t="s">
+    <row r="24" spans="3:12" ht="18.5" thickBot="1">
+      <c r="C24" t="s">
         <v>43</v>
       </c>
-      <c r="H21" t="s">
+      <c r="H24" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="3:12" ht="18.5" thickBot="1">
-      <c r="D22" s="5" t="s">
+    <row r="25" spans="3:12" ht="18.5" thickBot="1">
+      <c r="D25" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="E22" s="4">
+      <c r="E25" s="4">
         <v>1</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F25" t="s">
         <v>57</v>
       </c>
-      <c r="I22" s="5" t="s">
+      <c r="I25" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="J22" s="4">
+      <c r="J25" s="4">
         <v>9999</v>
       </c>
-      <c r="K22" t="s">
+      <c r="K25" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="23" spans="3:12" ht="18.5" thickBot="1">
-      <c r="D23" s="5" t="s">
+    <row r="26" spans="3:12" ht="18.5" thickBot="1">
+      <c r="D26" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="E23" s="4">
+      <c r="E26" s="4">
         <v>2</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F26" t="s">
         <v>58</v>
       </c>
-      <c r="I23" s="5" t="s">
+      <c r="I26" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="J23" s="4">
+      <c r="J26" s="4">
         <v>9999</v>
       </c>
-      <c r="K23" t="s">
+      <c r="K26" t="s">
         <v>56</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C13:K13"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="C9:D9"/>
     <mergeCell ref="C16:E16"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="H17:J17"/>
+    <mergeCell ref="C13:G13"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1501,8 +1601,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8435DF8B-284E-40B4-AEA6-EB65CAC52314}">
   <dimension ref="C2:L19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13:J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.58203125" defaultRowHeight="18"/>
@@ -1545,17 +1645,17 @@
       </c>
     </row>
     <row r="4" spans="3:12" ht="18.5" thickBot="1">
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="22"/>
-      <c r="I4" s="22"/>
-      <c r="J4" s="22"/>
-      <c r="K4" s="23"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="22"/>
       <c r="L4" t="s">
         <v>52</v>
       </c>

</xml_diff>